<commit_message>
Mudanças no arquivo .dss
</commit_message>
<xml_diff>
--- a/data/spreadsheets/sheet_IEEE13Node.xlsx
+++ b/data/spreadsheets/sheet_IEEE13Node.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2215373C-9A32-4458-AC5E-44392C64D18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250803A3-2B47-43B6-B018-01FBA09B641B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="123">
   <si>
     <t>Parameter</t>
   </si>
@@ -168,15 +168,9 @@
     <t>0.91</t>
   </si>
   <si>
-    <t>23</t>
-  </si>
-  <si>
     <t>MAC003983</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>MAC003996</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
     <t>MAC004000</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>MAC004000.csv</t>
   </si>
   <si>
@@ -406,6 +397,15 @@
   </si>
   <si>
     <t>pv_generation.csv</t>
+  </si>
+  <si>
+    <t>645_sec</t>
+  </si>
+  <si>
+    <t>670_sec</t>
+  </si>
+  <si>
+    <t>680_sec</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1000,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1044,8 +1044,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>645</v>
+      <c r="B2" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -1057,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -1076,8 +1076,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>670</v>
+      <c r="B3" t="s">
+        <v>121</v>
       </c>
       <c r="C3" s="2">
         <v>3</v>
@@ -1089,7 +1089,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -1098,7 +1098,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J3" s="2">
         <v>123</v>
@@ -1108,8 +1108,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>680</v>
+      <c r="B4" t="s">
+        <v>122</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1121,7 +1121,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J4" s="2">
         <v>123</v>
@@ -1153,13 +1153,13 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="8.88671875"/>
+    <col min="1" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="8.88671875"/>
     <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1206,7 +1206,7 @@
         <v>41</v>
       </c>
       <c r="B2">
-        <v>650</v>
+        <v>650001</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1232,8 +1232,8 @@
       <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
-        <v>43</v>
+      <c r="K2">
+        <v>234</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3">
-        <v>632</v>
+        <v>632001</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1270,8 +1270,8 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
-        <v>45</v>
+      <c r="K3">
+        <v>124</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -1279,10 +1279,10 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4">
-        <v>670</v>
+        <v>670001</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1308,8 +1308,8 @@
       <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
-        <v>45</v>
+      <c r="K4">
+        <v>124</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5">
-        <v>671</v>
+        <v>671001</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1346,8 +1346,8 @@
       <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="K5" t="s">
-        <v>45</v>
+      <c r="K5">
+        <v>124</v>
       </c>
       <c r="L5" t="s">
         <v>33</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>680</v>
+        <v>680001</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1384,8 +1384,8 @@
       <c r="J6" t="s">
         <v>25</v>
       </c>
-      <c r="K6" t="s">
-        <v>45</v>
+      <c r="K6">
+        <v>234</v>
       </c>
       <c r="L6" t="s">
         <v>36</v>
@@ -1393,10 +1393,10 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7">
-        <v>633</v>
+        <v>633001</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1422,19 +1422,19 @@
       <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="K7" t="s">
-        <v>50</v>
+      <c r="K7">
+        <v>134</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8">
-        <v>645</v>
+        <v>645001</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1460,19 +1460,19 @@
       <c r="J8" t="s">
         <v>25</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8">
+        <v>134</v>
+      </c>
+      <c r="L8" t="s">
         <v>50</v>
-      </c>
-      <c r="L8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B9">
-        <v>646</v>
+        <v>646001</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1498,19 +1498,19 @@
       <c r="J9" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
-        <v>45</v>
+      <c r="K9">
+        <v>124</v>
       </c>
       <c r="L9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10">
-        <v>692</v>
+        <v>692001</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1536,19 +1536,19 @@
       <c r="J10" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
-        <v>45</v>
+      <c r="K10">
+        <v>124</v>
       </c>
       <c r="L10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11">
-        <v>675</v>
+        <v>675001</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1574,19 +1574,19 @@
       <c r="J11" t="s">
         <v>25</v>
       </c>
-      <c r="K11" t="s">
-        <v>45</v>
+      <c r="K11">
+        <v>124</v>
       </c>
       <c r="L11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B12">
-        <v>684</v>
+        <v>684001</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1612,19 +1612,19 @@
       <c r="J12" t="s">
         <v>25</v>
       </c>
-      <c r="K12" t="s">
-        <v>45</v>
+      <c r="K12">
+        <v>134</v>
       </c>
       <c r="L12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13">
-        <v>611</v>
+        <v>611001</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H13">
         <v>8</v>
@@ -1650,19 +1650,19 @@
       <c r="J13" t="s">
         <v>25</v>
       </c>
-      <c r="K13" t="s">
-        <v>50</v>
+      <c r="K13">
+        <v>234</v>
       </c>
       <c r="L13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14">
-        <v>652</v>
+        <v>652001</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1688,19 +1688,19 @@
       <c r="J14" t="s">
         <v>25</v>
       </c>
-      <c r="K14" t="s">
-        <v>50</v>
+      <c r="K14">
+        <v>134</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15">
-        <v>650</v>
+        <v>650002</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1726,19 +1726,19 @@
       <c r="J15" t="s">
         <v>25</v>
       </c>
-      <c r="K15" t="s">
-        <v>50</v>
+      <c r="K15">
+        <v>124</v>
       </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16">
-        <v>632</v>
+        <v>632002</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1764,19 +1764,19 @@
       <c r="J16" t="s">
         <v>25</v>
       </c>
-      <c r="K16" t="s">
-        <v>50</v>
+      <c r="K16">
+        <v>234</v>
       </c>
       <c r="L16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17">
-        <v>670</v>
+        <v>670002</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1802,19 +1802,19 @@
       <c r="J17" t="s">
         <v>25</v>
       </c>
-      <c r="K17" t="s">
-        <v>50</v>
+      <c r="K17">
+        <v>134</v>
       </c>
       <c r="L17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B18">
-        <v>671</v>
+        <v>671002</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1840,19 +1840,19 @@
       <c r="J18" t="s">
         <v>25</v>
       </c>
-      <c r="K18" t="s">
-        <v>45</v>
+      <c r="K18">
+        <v>124</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B19">
-        <v>680</v>
+        <v>680002</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1878,19 +1878,19 @@
       <c r="J19" t="s">
         <v>25</v>
       </c>
-      <c r="K19" t="s">
-        <v>50</v>
+      <c r="K19">
+        <v>134</v>
       </c>
       <c r="L19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B20">
-        <v>633</v>
+        <v>633002</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1916,19 +1916,19 @@
       <c r="J20" t="s">
         <v>25</v>
       </c>
-      <c r="K20" t="s">
-        <v>43</v>
+      <c r="K20">
+        <v>234</v>
       </c>
       <c r="L20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B21">
-        <v>645</v>
+        <v>645002</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1954,19 +1954,19 @@
       <c r="J21" t="s">
         <v>25</v>
       </c>
-      <c r="K21" t="s">
-        <v>50</v>
+      <c r="K21">
+        <v>134</v>
       </c>
       <c r="L21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B22">
-        <v>646</v>
+        <v>646002</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1992,19 +1992,19 @@
       <c r="J22" t="s">
         <v>25</v>
       </c>
-      <c r="K22" t="s">
-        <v>50</v>
+      <c r="K22">
+        <v>134</v>
       </c>
       <c r="L22" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B23">
-        <v>692</v>
+        <v>692002</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2030,19 +2030,19 @@
       <c r="J23" t="s">
         <v>25</v>
       </c>
-      <c r="K23" t="s">
-        <v>45</v>
+      <c r="K23">
+        <v>124</v>
       </c>
       <c r="L23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B24">
-        <v>675</v>
+        <v>675002</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2068,19 +2068,19 @@
       <c r="J24" t="s">
         <v>25</v>
       </c>
-      <c r="K24" t="s">
-        <v>50</v>
+      <c r="K24">
+        <v>134</v>
       </c>
       <c r="L24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B25">
-        <v>684</v>
+        <v>684002</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2106,19 +2106,19 @@
       <c r="J25" t="s">
         <v>25</v>
       </c>
-      <c r="K25" t="s">
-        <v>43</v>
+      <c r="K25">
+        <v>234</v>
       </c>
       <c r="L25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B26">
-        <v>611</v>
+        <v>611002</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2144,19 +2144,19 @@
       <c r="J26" t="s">
         <v>25</v>
       </c>
-      <c r="K26" t="s">
-        <v>50</v>
+      <c r="K26">
+        <v>134</v>
       </c>
       <c r="L26" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B27">
-        <v>652</v>
+        <v>652002</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2182,19 +2182,19 @@
       <c r="J27" t="s">
         <v>25</v>
       </c>
-      <c r="K27" t="s">
-        <v>45</v>
+      <c r="K27">
+        <v>124</v>
       </c>
       <c r="L27" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B28">
-        <v>650</v>
+        <v>650003</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2220,19 +2220,19 @@
       <c r="J28" t="s">
         <v>25</v>
       </c>
-      <c r="K28" t="s">
-        <v>50</v>
+      <c r="K28">
+        <v>134</v>
       </c>
       <c r="L28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B29">
-        <v>632</v>
+        <v>632003</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2258,19 +2258,19 @@
       <c r="J29" t="s">
         <v>25</v>
       </c>
-      <c r="K29" t="s">
-        <v>43</v>
+      <c r="K29">
+        <v>234</v>
       </c>
       <c r="L29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B30">
-        <v>670</v>
+        <v>670003</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2296,19 +2296,19 @@
       <c r="J30" t="s">
         <v>25</v>
       </c>
-      <c r="K30" t="s">
-        <v>50</v>
+      <c r="K30">
+        <v>134</v>
       </c>
       <c r="L30" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B31">
-        <v>671</v>
+        <v>671003</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2334,19 +2334,19 @@
       <c r="J31" t="s">
         <v>25</v>
       </c>
-      <c r="K31" t="s">
-        <v>43</v>
+      <c r="K31">
+        <v>234</v>
       </c>
       <c r="L31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B32">
-        <v>680</v>
+        <v>680003</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2372,19 +2372,19 @@
       <c r="J32" t="s">
         <v>25</v>
       </c>
-      <c r="K32" t="s">
-        <v>43</v>
+      <c r="K32">
+        <v>234</v>
       </c>
       <c r="L32" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B33">
-        <v>633</v>
+        <v>633003</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2410,19 +2410,19 @@
       <c r="J33" t="s">
         <v>25</v>
       </c>
-      <c r="K33" t="s">
-        <v>43</v>
+      <c r="K33">
+        <v>234</v>
       </c>
       <c r="L33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B34">
-        <v>645</v>
+        <v>645003</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2448,19 +2448,19 @@
       <c r="J34" t="s">
         <v>25</v>
       </c>
-      <c r="K34" t="s">
-        <v>45</v>
+      <c r="K34">
+        <v>124</v>
       </c>
       <c r="L34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B35">
-        <v>646</v>
+        <v>646003</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2486,19 +2486,19 @@
       <c r="J35" t="s">
         <v>25</v>
       </c>
-      <c r="K35" t="s">
-        <v>43</v>
+      <c r="K35">
+        <v>234</v>
       </c>
       <c r="L35" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B36">
-        <v>692</v>
+        <v>692003</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2524,19 +2524,19 @@
       <c r="J36" t="s">
         <v>25</v>
       </c>
-      <c r="K36" t="s">
-        <v>45</v>
+      <c r="K36">
+        <v>124</v>
       </c>
       <c r="L36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B37">
-        <v>675</v>
+        <v>675003</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2562,19 +2562,19 @@
       <c r="J37" t="s">
         <v>25</v>
       </c>
-      <c r="K37" t="s">
-        <v>45</v>
+      <c r="K37">
+        <v>124</v>
       </c>
       <c r="L37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B38">
-        <v>684</v>
+        <v>684003</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2600,19 +2600,19 @@
       <c r="J38" t="s">
         <v>25</v>
       </c>
-      <c r="K38" t="s">
-        <v>50</v>
+      <c r="K38">
+        <v>134</v>
       </c>
       <c r="L38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B39">
-        <v>611</v>
+        <v>611003</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2638,19 +2638,19 @@
       <c r="J39" t="s">
         <v>25</v>
       </c>
-      <c r="K39" t="s">
-        <v>50</v>
+      <c r="K39">
+        <v>134</v>
       </c>
       <c r="L39" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B40">
-        <v>652</v>
+        <v>652003</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2676,19 +2676,19 @@
       <c r="J40" t="s">
         <v>25</v>
       </c>
-      <c r="K40" t="s">
-        <v>50</v>
+      <c r="K40">
+        <v>134</v>
       </c>
       <c r="L40" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B41">
-        <v>650</v>
+        <v>650004</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2714,11 +2714,11 @@
       <c r="J41" t="s">
         <v>25</v>
       </c>
-      <c r="K41" t="s">
-        <v>43</v>
+      <c r="K41">
+        <v>234</v>
       </c>
       <c r="L41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2815,7 +2815,7 @@
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2853,7 +2853,7 @@
         <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>23</v>
       </c>
       <c r="L5" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2967,7 +2967,7 @@
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3005,7 +3005,7 @@
         <v>23</v>
       </c>
       <c r="L7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3043,7 +3043,7 @@
         <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3119,7 +3119,7 @@
         <v>13</v>
       </c>
       <c r="L10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3157,7 +3157,7 @@
         <v>23</v>
       </c>
       <c r="L11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3195,7 +3195,7 @@
         <v>13</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3233,7 +3233,7 @@
         <v>23</v>
       </c>
       <c r="L13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3271,7 +3271,7 @@
         <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Organização dos arquivos para rodar novo fluxo 5 nós
</commit_message>
<xml_diff>
--- a/data/spreadsheets/sheet_IEEE13Node.xlsx
+++ b/data/spreadsheets/sheet_IEEE13Node.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250803A3-2B47-43B6-B018-01FBA09B641B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA99138-7D30-4399-A57C-0E63374CC226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="133">
   <si>
     <t>Parameter</t>
   </si>
@@ -406,6 +406,36 @@
   </si>
   <si>
     <t>680_sec</t>
+  </si>
+  <si>
+    <t>650_sec</t>
+  </si>
+  <si>
+    <t>632_sec</t>
+  </si>
+  <si>
+    <t>671_sec</t>
+  </si>
+  <si>
+    <t>633_sec</t>
+  </si>
+  <si>
+    <t>646_sec</t>
+  </si>
+  <si>
+    <t>692_sec</t>
+  </si>
+  <si>
+    <t>675_sec</t>
+  </si>
+  <si>
+    <t>684_sec</t>
+  </si>
+  <si>
+    <t>611_sec</t>
+  </si>
+  <si>
+    <t>652_sec</t>
   </si>
 </sst>
 </file>
@@ -905,7 +935,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -950,8 +980,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>4</v>
+      <c r="B2" t="s">
+        <v>123</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -999,8 +1029,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1152,8 +1182,8 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1205,8 +1235,8 @@
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2">
-        <v>650001</v>
+      <c r="B2" t="s">
+        <v>123</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1233,7 +1263,7 @@
         <v>25</v>
       </c>
       <c r="K2">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -1243,8 +1273,8 @@
       <c r="A3" t="s">
         <v>43</v>
       </c>
-      <c r="B3">
-        <v>632001</v>
+      <c r="B3" t="s">
+        <v>124</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1271,7 +1301,7 @@
         <v>25</v>
       </c>
       <c r="K3">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L3" t="s">
         <v>31</v>
@@ -1281,8 +1311,8 @@
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4">
-        <v>670001</v>
+      <c r="B4" t="s">
+        <v>121</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1309,7 +1339,7 @@
         <v>25</v>
       </c>
       <c r="K4">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
         <v>32</v>
@@ -1319,8 +1349,8 @@
       <c r="A5" t="s">
         <v>45</v>
       </c>
-      <c r="B5">
-        <v>671001</v>
+      <c r="B5" t="s">
+        <v>125</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1347,7 +1377,7 @@
         <v>25</v>
       </c>
       <c r="K5">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
         <v>33</v>
@@ -1357,8 +1387,8 @@
       <c r="A6" t="s">
         <v>46</v>
       </c>
-      <c r="B6">
-        <v>680001</v>
+      <c r="B6" t="s">
+        <v>122</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1385,7 +1415,7 @@
         <v>25</v>
       </c>
       <c r="K6">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
         <v>36</v>
@@ -1395,8 +1425,8 @@
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B7">
-        <v>633001</v>
+      <c r="B7" t="s">
+        <v>126</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -1423,7 +1453,7 @@
         <v>25</v>
       </c>
       <c r="K7">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L7" t="s">
         <v>48</v>
@@ -1433,8 +1463,8 @@
       <c r="A8" t="s">
         <v>49</v>
       </c>
-      <c r="B8">
-        <v>645001</v>
+      <c r="B8" t="s">
+        <v>120</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1461,7 +1491,7 @@
         <v>25</v>
       </c>
       <c r="K8">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
         <v>50</v>
@@ -1471,8 +1501,8 @@
       <c r="A9" t="s">
         <v>51</v>
       </c>
-      <c r="B9">
-        <v>646001</v>
+      <c r="B9" t="s">
+        <v>127</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -1499,7 +1529,7 @@
         <v>25</v>
       </c>
       <c r="K9">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
         <v>52</v>
@@ -1509,8 +1539,8 @@
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10">
-        <v>692001</v>
+      <c r="B10" t="s">
+        <v>128</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1537,7 +1567,7 @@
         <v>25</v>
       </c>
       <c r="K10">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
         <v>54</v>
@@ -1547,8 +1577,8 @@
       <c r="A11" t="s">
         <v>55</v>
       </c>
-      <c r="B11">
-        <v>675001</v>
+      <c r="B11" t="s">
+        <v>129</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1575,7 +1605,7 @@
         <v>25</v>
       </c>
       <c r="K11">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L11" t="s">
         <v>56</v>
@@ -1585,8 +1615,8 @@
       <c r="A12" t="s">
         <v>57</v>
       </c>
-      <c r="B12">
-        <v>684001</v>
+      <c r="B12" t="s">
+        <v>130</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1613,7 +1643,7 @@
         <v>25</v>
       </c>
       <c r="K12">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L12" t="s">
         <v>58</v>
@@ -1623,8 +1653,8 @@
       <c r="A13" t="s">
         <v>59</v>
       </c>
-      <c r="B13">
-        <v>611001</v>
+      <c r="B13" t="s">
+        <v>131</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1651,7 +1681,7 @@
         <v>25</v>
       </c>
       <c r="K13">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L13" t="s">
         <v>61</v>
@@ -1661,8 +1691,8 @@
       <c r="A14" t="s">
         <v>62</v>
       </c>
-      <c r="B14">
-        <v>652001</v>
+      <c r="B14" t="s">
+        <v>132</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1689,7 +1719,7 @@
         <v>25</v>
       </c>
       <c r="K14">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L14" t="s">
         <v>63</v>
@@ -1699,8 +1729,8 @@
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15">
-        <v>650002</v>
+      <c r="B15" t="s">
+        <v>123</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1727,7 +1757,7 @@
         <v>25</v>
       </c>
       <c r="K15">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L15" t="s">
         <v>65</v>
@@ -1737,8 +1767,8 @@
       <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="B16">
-        <v>632002</v>
+      <c r="B16" t="s">
+        <v>124</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1765,7 +1795,7 @@
         <v>25</v>
       </c>
       <c r="K16">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L16" t="s">
         <v>67</v>
@@ -1775,8 +1805,8 @@
       <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17">
-        <v>670002</v>
+      <c r="B17" t="s">
+        <v>121</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1803,7 +1833,7 @@
         <v>25</v>
       </c>
       <c r="K17">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L17" t="s">
         <v>69</v>
@@ -1813,8 +1843,8 @@
       <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B18">
-        <v>671002</v>
+      <c r="B18" t="s">
+        <v>125</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1841,7 +1871,7 @@
         <v>25</v>
       </c>
       <c r="K18">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L18" t="s">
         <v>71</v>
@@ -1851,8 +1881,8 @@
       <c r="A19" t="s">
         <v>72</v>
       </c>
-      <c r="B19">
-        <v>680002</v>
+      <c r="B19" t="s">
+        <v>122</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1879,7 +1909,7 @@
         <v>25</v>
       </c>
       <c r="K19">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L19" t="s">
         <v>73</v>
@@ -1889,8 +1919,8 @@
       <c r="A20" t="s">
         <v>74</v>
       </c>
-      <c r="B20">
-        <v>633002</v>
+      <c r="B20" t="s">
+        <v>126</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1917,7 +1947,7 @@
         <v>25</v>
       </c>
       <c r="K20">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L20" t="s">
         <v>75</v>
@@ -1927,8 +1957,8 @@
       <c r="A21" t="s">
         <v>76</v>
       </c>
-      <c r="B21">
-        <v>645002</v>
+      <c r="B21" t="s">
+        <v>120</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1955,7 +1985,7 @@
         <v>25</v>
       </c>
       <c r="K21">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L21" t="s">
         <v>77</v>
@@ -1965,8 +1995,8 @@
       <c r="A22" t="s">
         <v>78</v>
       </c>
-      <c r="B22">
-        <v>646002</v>
+      <c r="B22" t="s">
+        <v>127</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1993,7 +2023,7 @@
         <v>25</v>
       </c>
       <c r="K22">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L22" t="s">
         <v>79</v>
@@ -2003,8 +2033,8 @@
       <c r="A23" t="s">
         <v>80</v>
       </c>
-      <c r="B23">
-        <v>692002</v>
+      <c r="B23" t="s">
+        <v>128</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2031,7 +2061,7 @@
         <v>25</v>
       </c>
       <c r="K23">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L23" t="s">
         <v>81</v>
@@ -2041,8 +2071,8 @@
       <c r="A24" t="s">
         <v>82</v>
       </c>
-      <c r="B24">
-        <v>675002</v>
+      <c r="B24" t="s">
+        <v>129</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -2069,7 +2099,7 @@
         <v>25</v>
       </c>
       <c r="K24">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L24" t="s">
         <v>83</v>
@@ -2079,8 +2109,8 @@
       <c r="A25" t="s">
         <v>84</v>
       </c>
-      <c r="B25">
-        <v>684002</v>
+      <c r="B25" t="s">
+        <v>130</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2107,7 +2137,7 @@
         <v>25</v>
       </c>
       <c r="K25">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L25" t="s">
         <v>85</v>
@@ -2117,8 +2147,8 @@
       <c r="A26" t="s">
         <v>86</v>
       </c>
-      <c r="B26">
-        <v>611002</v>
+      <c r="B26" t="s">
+        <v>131</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -2145,7 +2175,7 @@
         <v>25</v>
       </c>
       <c r="K26">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L26" t="s">
         <v>87</v>
@@ -2155,8 +2185,8 @@
       <c r="A27" t="s">
         <v>88</v>
       </c>
-      <c r="B27">
-        <v>652002</v>
+      <c r="B27" t="s">
+        <v>132</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -2183,7 +2213,7 @@
         <v>25</v>
       </c>
       <c r="K27">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L27" t="s">
         <v>89</v>
@@ -2193,8 +2223,8 @@
       <c r="A28" t="s">
         <v>90</v>
       </c>
-      <c r="B28">
-        <v>650003</v>
+      <c r="B28" t="s">
+        <v>123</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -2221,7 +2251,7 @@
         <v>25</v>
       </c>
       <c r="K28">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L28" t="s">
         <v>91</v>
@@ -2231,8 +2261,8 @@
       <c r="A29" t="s">
         <v>92</v>
       </c>
-      <c r="B29">
-        <v>632003</v>
+      <c r="B29" t="s">
+        <v>124</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -2259,7 +2289,7 @@
         <v>25</v>
       </c>
       <c r="K29">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L29" t="s">
         <v>93</v>
@@ -2269,8 +2299,8 @@
       <c r="A30" t="s">
         <v>94</v>
       </c>
-      <c r="B30">
-        <v>670003</v>
+      <c r="B30" t="s">
+        <v>121</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -2297,7 +2327,7 @@
         <v>25</v>
       </c>
       <c r="K30">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L30" t="s">
         <v>95</v>
@@ -2307,8 +2337,8 @@
       <c r="A31" t="s">
         <v>96</v>
       </c>
-      <c r="B31">
-        <v>671003</v>
+      <c r="B31" t="s">
+        <v>125</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -2335,7 +2365,7 @@
         <v>25</v>
       </c>
       <c r="K31">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L31" t="s">
         <v>97</v>
@@ -2345,8 +2375,8 @@
       <c r="A32" t="s">
         <v>98</v>
       </c>
-      <c r="B32">
-        <v>680003</v>
+      <c r="B32" t="s">
+        <v>122</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2373,7 +2403,7 @@
         <v>25</v>
       </c>
       <c r="K32">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L32" t="s">
         <v>99</v>
@@ -2383,8 +2413,8 @@
       <c r="A33" t="s">
         <v>100</v>
       </c>
-      <c r="B33">
-        <v>633003</v>
+      <c r="B33" t="s">
+        <v>126</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -2411,7 +2441,7 @@
         <v>25</v>
       </c>
       <c r="K33">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L33" t="s">
         <v>101</v>
@@ -2421,8 +2451,8 @@
       <c r="A34" t="s">
         <v>102</v>
       </c>
-      <c r="B34">
-        <v>645003</v>
+      <c r="B34" t="s">
+        <v>120</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2449,7 +2479,7 @@
         <v>25</v>
       </c>
       <c r="K34">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L34" t="s">
         <v>103</v>
@@ -2459,8 +2489,8 @@
       <c r="A35" t="s">
         <v>104</v>
       </c>
-      <c r="B35">
-        <v>646003</v>
+      <c r="B35" t="s">
+        <v>127</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -2487,7 +2517,7 @@
         <v>25</v>
       </c>
       <c r="K35">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L35" t="s">
         <v>105</v>
@@ -2497,8 +2527,8 @@
       <c r="A36" t="s">
         <v>106</v>
       </c>
-      <c r="B36">
-        <v>692003</v>
+      <c r="B36" t="s">
+        <v>128</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -2525,7 +2555,7 @@
         <v>25</v>
       </c>
       <c r="K36">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L36" t="s">
         <v>107</v>
@@ -2535,8 +2565,8 @@
       <c r="A37" t="s">
         <v>108</v>
       </c>
-      <c r="B37">
-        <v>675003</v>
+      <c r="B37" t="s">
+        <v>129</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2563,7 +2593,7 @@
         <v>25</v>
       </c>
       <c r="K37">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="L37" t="s">
         <v>109</v>
@@ -2573,8 +2603,8 @@
       <c r="A38" t="s">
         <v>110</v>
       </c>
-      <c r="B38">
-        <v>684003</v>
+      <c r="B38" t="s">
+        <v>130</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2601,7 +2631,7 @@
         <v>25</v>
       </c>
       <c r="K38">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L38" t="s">
         <v>111</v>
@@ -2611,8 +2641,8 @@
       <c r="A39" t="s">
         <v>112</v>
       </c>
-      <c r="B39">
-        <v>611003</v>
+      <c r="B39" t="s">
+        <v>131</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -2639,7 +2669,7 @@
         <v>25</v>
       </c>
       <c r="K39">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L39" t="s">
         <v>113</v>
@@ -2649,8 +2679,8 @@
       <c r="A40" t="s">
         <v>114</v>
       </c>
-      <c r="B40">
-        <v>652003</v>
+      <c r="B40" t="s">
+        <v>132</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2677,7 +2707,7 @@
         <v>25</v>
       </c>
       <c r="K40">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="L40" t="s">
         <v>115</v>
@@ -2687,8 +2717,8 @@
       <c r="A41" t="s">
         <v>116</v>
       </c>
-      <c r="B41">
-        <v>650004</v>
+      <c r="B41" t="s">
+        <v>123</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2715,7 +2745,7 @@
         <v>25</v>
       </c>
       <c r="K41">
-        <v>234</v>
+        <v>23</v>
       </c>
       <c r="L41" t="s">
         <v>117</v>
@@ -2732,7 +2762,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2784,8 +2814,8 @@
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="B2">
-        <v>650</v>
+      <c r="B2" t="s">
+        <v>123</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2822,8 +2852,8 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3">
-        <v>632</v>
+      <c r="B3" t="s">
+        <v>124</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2860,8 +2890,8 @@
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4">
-        <v>670</v>
+      <c r="B4" t="s">
+        <v>121</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2898,8 +2928,8 @@
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5">
-        <v>671</v>
+      <c r="B5" t="s">
+        <v>125</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2936,8 +2966,8 @@
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6">
-        <v>680</v>
+      <c r="B6" t="s">
+        <v>122</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -2974,8 +3004,8 @@
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7">
-        <v>633</v>
+      <c r="B7" t="s">
+        <v>126</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -3012,8 +3042,8 @@
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8">
-        <v>645</v>
+      <c r="B8" t="s">
+        <v>120</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3050,8 +3080,8 @@
       <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="B9">
-        <v>646</v>
+      <c r="B9" t="s">
+        <v>127</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -3088,8 +3118,8 @@
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10">
-        <v>692</v>
+      <c r="B10" t="s">
+        <v>128</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -3126,8 +3156,8 @@
       <c r="A11" t="s">
         <v>38</v>
       </c>
-      <c r="B11">
-        <v>675</v>
+      <c r="B11" t="s">
+        <v>129</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -3164,8 +3194,8 @@
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12">
-        <v>684</v>
+      <c r="B12" t="s">
+        <v>130</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -3202,8 +3232,8 @@
       <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B13">
-        <v>611</v>
+      <c r="B13" t="s">
+        <v>131</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3240,8 +3270,8 @@
       <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B14">
-        <v>652</v>
+      <c r="B14" t="s">
+        <v>132</v>
       </c>
       <c r="C14">
         <v>1</v>

</xml_diff>